<commit_message>
alter notebook columns of dataframe and bar chart
</commit_message>
<xml_diff>
--- a/experiments/experiment_2/notebooks/estrategia1.xlsx
+++ b/experiments/experiment_2/notebooks/estrategia1.xlsx
@@ -561,7 +561,7 @@
         <v>10</v>
       </c>
       <c r="E2">
-        <v>14.3</v>
+        <v>14.29</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -594,13 +594,13 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="S2">
         <v>25</v>
@@ -609,7 +609,7 @@
         <v>10</v>
       </c>
       <c r="U2">
-        <v>14.3</v>
+        <v>14.29</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -668,7 +668,7 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q3">
         <v>0</v>
@@ -742,13 +742,13 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>0</v>
+        <v>294</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S4">
         <v>0</v>
@@ -777,13 +777,13 @@
         <v>26</v>
       </c>
       <c r="C5">
-        <v>2.4</v>
+        <v>2.41</v>
       </c>
       <c r="D5">
         <v>30</v>
       </c>
       <c r="E5">
-        <v>4.5</v>
+        <v>4.46</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -816,22 +816,22 @@
         <v>2</v>
       </c>
       <c r="P5">
-        <v>0</v>
+        <v>245</v>
       </c>
       <c r="Q5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R5">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S5">
-        <v>2.4</v>
+        <v>2.41</v>
       </c>
       <c r="T5">
         <v>30</v>
       </c>
       <c r="U5">
-        <v>4.5</v>
+        <v>4.46</v>
       </c>
       <c r="V5">
         <v>0.008032128514056224</v>
@@ -851,13 +851,13 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>2.4</v>
+        <v>2.38</v>
       </c>
       <c r="D6">
         <v>25</v>
       </c>
       <c r="E6">
-        <v>4.3</v>
+        <v>4.35</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -890,22 +890,22 @@
         <v>3</v>
       </c>
       <c r="P6">
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="R6">
         <v>0</v>
       </c>
       <c r="S6">
-        <v>2.4</v>
+        <v>2.38</v>
       </c>
       <c r="T6">
         <v>25</v>
       </c>
       <c r="U6">
-        <v>4.3</v>
+        <v>4.35</v>
       </c>
       <c r="V6">
         <v>0.01428571428571429</v>
@@ -925,13 +925,13 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <v>0.8</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="D7">
         <v>5</v>
       </c>
       <c r="E7">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -964,22 +964,22 @@
         <v>0</v>
       </c>
       <c r="P7">
-        <v>0</v>
+        <v>115</v>
       </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S7">
-        <v>0.8</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="T7">
         <v>5</v>
       </c>
       <c r="U7">
-        <v>1.4</v>
+        <v>1.39</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -999,13 +999,13 @@
         <v>29</v>
       </c>
       <c r="C8">
-        <v>9.1</v>
+        <v>9.09</v>
       </c>
       <c r="D8">
         <v>35</v>
       </c>
       <c r="E8">
-        <v>14.4</v>
+        <v>14.43</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1038,22 +1038,22 @@
         <v>2</v>
       </c>
       <c r="P8">
-        <v>0</v>
+        <v>68</v>
       </c>
       <c r="Q8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="R8">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="S8">
-        <v>9.1</v>
+        <v>9.09</v>
       </c>
       <c r="T8">
         <v>35</v>
       </c>
       <c r="U8">
-        <v>14.4</v>
+        <v>14.43</v>
       </c>
       <c r="V8">
         <v>0.02597402597402598</v>
@@ -1115,13 +1115,13 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>1.8</v>
+        <v>1.82</v>
       </c>
       <c r="T9">
         <v>85</v>
       </c>
       <c r="U9">
-        <v>3.6</v>
+        <v>3.56</v>
       </c>
       <c r="V9">
         <v>0.00748663101604278</v>

</xml_diff>

<commit_message>
dataframe, chart and styles to visualize
</commit_message>
<xml_diff>
--- a/experiments/experiment_2/notebooks/estrategia1.xlsx
+++ b/experiments/experiment_2/notebooks/estrategia1.xlsx
@@ -85,25 +85,25 @@
     <t>final_accumulated_fmeasure</t>
   </si>
   <si>
+    <t>wiley</t>
+  </si>
+  <si>
+    <t>webofscience</t>
+  </si>
+  <si>
+    <t>springer</t>
+  </si>
+  <si>
+    <t>scopus</t>
+  </si>
+  <si>
+    <t>sciencedirect</t>
+  </si>
+  <si>
     <t>elcompendex</t>
   </si>
   <si>
-    <t>webofscience</t>
-  </si>
-  <si>
-    <t>wiley</t>
-  </si>
-  <si>
-    <t>sciencedirect</t>
-  </si>
-  <si>
     <t>acm</t>
-  </si>
-  <si>
-    <t>springer</t>
-  </si>
-  <si>
-    <t>scopus</t>
   </si>
   <si>
     <t>s0</t>
@@ -555,13 +555,13 @@
         <v>23</v>
       </c>
       <c r="C2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>14.29</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -576,40 +576,40 @@
         <v>31</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>8</v>
+        <v>295</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>8</v>
+        <v>295</v>
       </c>
       <c r="O2">
         <v>0</v>
       </c>
       <c r="P2">
+        <v>294</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
         <v>1</v>
       </c>
-      <c r="Q2">
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <v>7</v>
-      </c>
       <c r="S2">
-        <v>25</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>14.29</v>
+        <v>0</v>
       </c>
       <c r="V2">
         <v>0</v>
@@ -703,13 +703,13 @@
         <v>25</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1.39</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -724,40 +724,40 @@
         <v>31</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
-        <v>295</v>
+        <v>124</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
-        <v>295</v>
+        <v>124</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
-        <v>294</v>
+        <v>115</v>
       </c>
       <c r="Q4">
         <v>0</v>
       </c>
       <c r="R4">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="S4">
-        <v>0</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="T4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1.39</v>
       </c>
       <c r="V4">
         <v>0</v>
@@ -777,13 +777,13 @@
         <v>26</v>
       </c>
       <c r="C5">
-        <v>2.41</v>
+        <v>9.09</v>
       </c>
       <c r="D5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="E5">
-        <v>4.46</v>
+        <v>14.43</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -798,49 +798,49 @@
         <v>31</v>
       </c>
       <c r="J5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K5">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="N5">
-        <v>249</v>
+        <v>77</v>
       </c>
       <c r="O5">
         <v>2</v>
       </c>
       <c r="P5">
-        <v>245</v>
+        <v>68</v>
       </c>
       <c r="Q5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="R5">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="S5">
-        <v>2.41</v>
+        <v>9.09</v>
       </c>
       <c r="T5">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="U5">
-        <v>4.46</v>
+        <v>14.43</v>
       </c>
       <c r="V5">
-        <v>0.008032128514056224</v>
+        <v>0.02597402597402598</v>
       </c>
       <c r="W5">
         <v>0.25</v>
       </c>
       <c r="X5">
-        <v>0.01556420233463035</v>
+        <v>0.04705882352941176</v>
       </c>
     </row>
     <row r="6" spans="1:24">
@@ -851,13 +851,13 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>2.38</v>
+        <v>2.41</v>
       </c>
       <c r="D6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E6">
-        <v>4.35</v>
+        <v>4.46</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -872,49 +872,49 @@
         <v>31</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P6">
-        <v>210</v>
+        <v>245</v>
       </c>
       <c r="Q6">
         <v>5</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="S6">
-        <v>2.38</v>
+        <v>2.41</v>
       </c>
       <c r="T6">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="U6">
-        <v>4.35</v>
+        <v>4.46</v>
       </c>
       <c r="V6">
-        <v>0.01428571428571429</v>
+        <v>0.008032128514056224</v>
       </c>
       <c r="W6">
-        <v>0.375</v>
+        <v>0.25</v>
       </c>
       <c r="X6">
-        <v>0.02752293577981652</v>
+        <v>0.01556420233463035</v>
       </c>
     </row>
     <row r="7" spans="1:24">
@@ -925,13 +925,13 @@
         <v>28</v>
       </c>
       <c r="C7">
-        <v>0.8099999999999999</v>
+        <v>25</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E7">
-        <v>1.39</v>
+        <v>14.29</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -946,40 +946,40 @@
         <v>31</v>
       </c>
       <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>2</v>
+      </c>
+      <c r="N7">
+        <v>8</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
         <v>1</v>
       </c>
-      <c r="K7">
-        <v>124</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>124</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>115</v>
-      </c>
       <c r="Q7">
         <v>0</v>
       </c>
       <c r="R7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S7">
-        <v>0.8099999999999999</v>
+        <v>25</v>
       </c>
       <c r="T7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="U7">
-        <v>1.39</v>
+        <v>14.29</v>
       </c>
       <c r="V7">
         <v>0</v>
@@ -999,13 +999,13 @@
         <v>29</v>
       </c>
       <c r="C8">
-        <v>9.09</v>
+        <v>2.38</v>
       </c>
       <c r="D8">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="E8">
-        <v>14.43</v>
+        <v>4.35</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -1020,49 +1020,49 @@
         <v>31</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K8">
-        <v>77</v>
+        <v>210</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N8">
-        <v>77</v>
+        <v>210</v>
       </c>
       <c r="O8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <v>68</v>
+        <v>210</v>
       </c>
       <c r="Q8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="R8">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="S8">
-        <v>9.09</v>
+        <v>2.38</v>
       </c>
       <c r="T8">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="U8">
-        <v>14.43</v>
+        <v>4.35</v>
       </c>
       <c r="V8">
-        <v>0.02597402597402598</v>
+        <v>0.01428571428571429</v>
       </c>
       <c r="W8">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="X8">
-        <v>0.04705882352941176</v>
+        <v>0.02752293577981652</v>
       </c>
     </row>
     <row r="9" spans="1:24">

</xml_diff>

<commit_message>
add diag venn seed set
</commit_message>
<xml_diff>
--- a/experiments/experiment_2/notebooks/estrategia1.xlsx
+++ b/experiments/experiment_2/notebooks/estrategia1.xlsx
@@ -851,13 +851,13 @@
         <v>27</v>
       </c>
       <c r="C6">
-        <v>2.41</v>
+        <v>2.01</v>
       </c>
       <c r="D6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E6">
-        <v>4.46</v>
+        <v>3.72</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -872,7 +872,7 @@
         <v>31</v>
       </c>
       <c r="J6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>249</v>
@@ -881,7 +881,7 @@
         <v>0</v>
       </c>
       <c r="M6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N6">
         <v>249</v>
@@ -893,19 +893,19 @@
         <v>245</v>
       </c>
       <c r="Q6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="R6">
         <v>4</v>
       </c>
       <c r="S6">
-        <v>2.41</v>
+        <v>2.01</v>
       </c>
       <c r="T6">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="U6">
-        <v>4.46</v>
+        <v>3.72</v>
       </c>
       <c r="V6">
         <v>0.008032128514056224</v>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="N9">
         <v>935</v>
@@ -1115,13 +1115,13 @@
         <v>0</v>
       </c>
       <c r="S9">
-        <v>1.82</v>
+        <v>1.71</v>
       </c>
       <c r="T9">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="U9">
-        <v>3.56</v>
+        <v>3.35</v>
       </c>
       <c r="V9">
         <v>0.00748663101604278</v>

</xml_diff>